<commit_message>
Added Read Functionality and published to Orchestrator
</commit_message>
<xml_diff>
--- a/ConnectedOfiice Webapp User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/ConnectedOfiice Webapp User Acceptance Testing/Connected Office Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaryadev\Desktop\UNI\AARYADEV-STUDY\3rd Year\CMPG-323-Project-4-35553367\ConnectedOfiice Webapp User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F03E6337-24EA-4995-8CE2-4FAC7BA32B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CA39B2-6F14-4178-9109-90C469EB2C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>Status</t>
   </si>
@@ -290,9 +290,6 @@
   </si>
   <si>
     <t>Delete Test Passed</t>
-  </si>
-  <si>
-    <t>There is a bug with the update, on clicking save the Item is deleted, Cannot confirm if it is updated</t>
   </si>
 </sst>
 </file>
@@ -1128,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,10 +1167,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1187,10 +1184,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1204,10 +1201,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1221,10 +1218,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,10 +1235,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1255,10 +1252,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1272,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
         <v>0</v>
@@ -1289,7 +1286,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
         <v>0</v>
@@ -1306,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
         <v>0</v>
@@ -1323,10 +1320,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1340,10 +1337,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,10 +1354,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1374,7 +1371,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
         <v>0</v>
@@ -1391,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
         <v>0</v>
@@ -1402,16 +1399,16 @@
         <v>48</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,16 +1416,16 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,16 +1433,16 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,16 +1450,16 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1470,16 +1467,16 @@
         <v>52</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,16 +1484,16 @@
         <v>53</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,13 +1501,13 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
         <v>0</v>
@@ -1521,13 +1518,13 @@
         <v>55</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
         <v>0</v>
@@ -1538,21 +1535,16 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>